<commit_message>
merged last working version
</commit_message>
<xml_diff>
--- a/src/scenarios/scenario1.xlsx
+++ b/src/scenarios/scenario1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gustavo\stochastic\src\scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Doktorarbeit\UCC\OptiFramework\stochastic\src\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10470" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51600" windowHeight="17835"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -74,8 +74,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -356,173 +357,225 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.125</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>0.125</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.16666666666666666</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.20833333333333334</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.25</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>0</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.29166666666666669</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>0</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.33333333333333331</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.375</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -533,13 +586,19 @@
       <c r="E10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>0</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.41666666666666669</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -550,13 +609,19 @@
       <c r="E11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>0</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.45833333333333331</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -567,13 +632,19 @@
       <c r="E12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>0</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.5</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -584,13 +655,19 @@
       <c r="E13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>0</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.54166666666666663</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -601,13 +678,19 @@
       <c r="E14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>0</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.58333333333333337</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -618,13 +701,19 @@
       <c r="E15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>0</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.625</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -635,13 +724,19 @@
       <c r="E16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>0</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.66666666666666663</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -652,13 +747,19 @@
       <c r="E17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>0</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.70833333333333337</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -669,13 +770,19 @@
       <c r="E18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>0</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.75</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -686,13 +793,19 @@
       <c r="E19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>0</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.79166666666666663</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -703,89 +816,125 @@
       <c r="E20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21">
-        <v>2</v>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.83333333333333337</v>
       </c>
       <c r="C21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D21">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E21">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>1</v>
-      </c>
-      <c r="B22">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="F21">
+        <v>4</v>
+      </c>
+      <c r="G21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.875</v>
       </c>
       <c r="C22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E22">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="F22">
+        <v>4</v>
+      </c>
+      <c r="G22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.91666666666666663</v>
       </c>
       <c r="C23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E23">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>1</v>
-      </c>
-      <c r="B24">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <v>4</v>
+      </c>
+      <c r="G23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.95833333333333337</v>
       </c>
       <c r="C24">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E24">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>1</v>
-      </c>
-      <c r="B25">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="F24">
+        <v>4</v>
+      </c>
+      <c r="G24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0</v>
       </c>
       <c r="C25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D25">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25">
+        <v>4</v>
+      </c>
+      <c r="G25">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
latest version with amd
</commit_message>
<xml_diff>
--- a/src/scenarios/scenario1.xlsx
+++ b/src/scenarios/scenario1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Doktorarbeit\UCC\OptiFramework\stochastic\src\scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Doktorarbeit\UCC\Linksmart\stochastic-simulator-paper\src\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,19 +26,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Car1</t>
+    <t>charger1</t>
   </si>
   <si>
-    <t>Car2</t>
+    <t>charger2</t>
   </si>
   <si>
-    <t>Car3</t>
+    <t>charger3</t>
   </si>
   <si>
-    <t>Car4</t>
+    <t>charger4</t>
   </si>
   <si>
-    <t>Car5</t>
+    <t>charger5</t>
   </si>
 </sst>
 </file>
@@ -360,7 +360,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>